<commit_message>
Updated most parts to support categories without children
</commit_message>
<xml_diff>
--- a/test/data/products_test.xlsx
+++ b/test/data/products_test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasosterle/Documents/code/WEB/react-cintamani/cintamani-next/test/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oesiw\Documents\code\cintamani\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33040" yWindow="-60" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33045" yWindow="-60" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Thangkas - big Tsagil</t>
+  </si>
+  <si>
+    <t>Klangschalen</t>
+  </si>
+  <si>
+    <t>Testschale</t>
+  </si>
+  <si>
+    <t>KKS003.JPG</t>
+  </si>
+  <si>
+    <t>Klangschale beschreibung</t>
   </si>
 </sst>
 </file>
@@ -436,23 +448,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -498,7 +510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -544,7 +556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -565,6 +577,29 @@
       </c>
       <c r="G5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>